<commit_message>
Add useful information for the error message
</commit_message>
<xml_diff>
--- a/samples/idaithalam-excel-apitesting/src/test/resources/virtualan_collection_testcase_8.xlsx
+++ b/samples/idaithalam-excel-apitesting/src/test/resources/virtualan_collection_testcase_8.xlsx
@@ -776,7 +776,7 @@
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="topLeft" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="14.43" defaultRowHeight="15"/>
@@ -866,9 +866,7 @@
       <c r="L2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="M2" s="1"/>
       <c r="N2" s="1" t="s">
         <v>25</v>
       </c>
@@ -948,7 +946,6 @@
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="M2" r:id="rId2"/>
     <hyperlink ref="C3" r:id="rId3"/>
     <hyperlink ref="C4" r:id="rId4"/>
   </hyperlinks>

</xml_diff>